<commit_message>
cleaned up exp directories and reran sims
</commit_message>
<xml_diff>
--- a/experimental_runs/1_freeDecay/flapDecay/WECSIM_exp5_flap1Decay.xlsx
+++ b/experimental_runs/1_freeDecay/flapDecay/WECSIM_exp5_flap1Decay.xlsx
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Log!$B$1:$G$22</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -84,37 +84,6 @@
         <color theme="1"/>
         <rFont val="Helvetica"/>
       </rPr>
-      <t>=0.91</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>°</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>θ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>i</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Helvetica"/>
-      </rPr>
       <t>=0.4°</t>
     </r>
   </si>
@@ -353,6 +322,37 @@
   <si>
     <t>FAILED: ran out of time</t>
   </si>
+  <si>
+    <r>
+      <t>θ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>=0.91</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>°, Omit, little decay</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -363,7 +363,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -422,14 +422,25 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <color rgb="FFFF0000"/>
+      <name val="Helvetica"/>
       <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Helvetica"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1543,7 +1554,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1645,19 +1656,19 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1718,6 +1729,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="773">
@@ -2833,7 +2859,7 @@
   <dimension ref="B1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2894,7 +2920,7 @@
       <c r="B4" s="3"/>
       <c r="D4"/>
       <c r="E4" s="28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -2927,7 +2953,7 @@
     </row>
     <row r="7" spans="2:10" s="25" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="44" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="45"/>
       <c r="D7" s="45"/>
@@ -2940,7 +2966,7 @@
     </row>
     <row r="8" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="47" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="24"/>
       <c r="D8" s="24"/>
@@ -2953,7 +2979,7 @@
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B9" s="47" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
@@ -2966,7 +2992,7 @@
     </row>
     <row r="10" spans="2:10" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B10" s="47" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" s="50"/>
       <c r="D10" s="50"/>
@@ -2979,7 +3005,7 @@
     </row>
     <row r="11" spans="2:10" s="25" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="52" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="53"/>
       <c r="D11" s="53"/>
@@ -3006,7 +3032,7 @@
         <v>0</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E13" s="31" t="s">
         <v>3</v>
@@ -3022,18 +3048,18 @@
       <c r="B14" s="57">
         <v>1</v>
       </c>
-      <c r="C14" s="33">
+      <c r="C14" s="65">
         <v>1</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="66">
         <v>3</v>
       </c>
-      <c r="E14" s="36">
+      <c r="E14" s="67">
         <v>42342</v>
       </c>
-      <c r="F14" s="17"/>
-      <c r="G14" s="18" t="s">
-        <v>14</v>
+      <c r="F14" s="68"/>
+      <c r="G14" s="69" t="s">
+        <v>30</v>
       </c>
       <c r="H14" s="11"/>
       <c r="I14" s="12"/>
@@ -3053,7 +3079,7 @@
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H15" s="11"/>
       <c r="I15" s="13"/>
@@ -3073,7 +3099,7 @@
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H16" s="11"/>
       <c r="I16" s="13"/>
@@ -3093,7 +3119,7 @@
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -3110,7 +3136,7 @@
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
@@ -3127,7 +3153,7 @@
       </c>
       <c r="F19" s="42"/>
       <c r="G19" s="43" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -3144,7 +3170,7 @@
       </c>
       <c r="F20" s="21"/>
       <c r="G20" s="22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -3163,7 +3189,7 @@
       </c>
       <c r="F21" s="17"/>
       <c r="G21" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -3180,7 +3206,7 @@
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -3197,7 +3223,7 @@
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -3214,7 +3240,7 @@
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -3231,7 +3257,7 @@
       </c>
       <c r="F25" s="21"/>
       <c r="G25" s="22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -3250,7 +3276,7 @@
       </c>
       <c r="F26" s="17"/>
       <c r="G26" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -3267,7 +3293,7 @@
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -3284,7 +3310,7 @@
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="2:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -3301,7 +3327,7 @@
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -3318,7 +3344,7 @@
       </c>
       <c r="F30" s="21"/>
       <c r="G30" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="2:7" ht="15.75" x14ac:dyDescent="0.3">
@@ -3337,7 +3363,7 @@
       </c>
       <c r="F31" s="17"/>
       <c r="G31" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>